<commit_message>
Elements and Weapons as Many2one model
</commit_message>
<xml_diff>
--- a/personajes.xlsx
+++ b/personajes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OdooCDev\custom\genshin_impact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A3D3FD-9B2C-487F-A6BB-C7F2C42B9BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4268D05A-F294-45C2-9790-5AFEEAAE5186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15780" yWindow="555" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.42578125" defaultRowHeight="15"/>
@@ -595,10 +595,10 @@
         <v>52</v>
       </c>
       <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
         <v>51</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
       </c>
       <c r="G1" t="s">
         <v>50</v>
@@ -618,7 +618,7 @@
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -650,7 +650,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -682,7 +682,7 @@
         <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -714,7 +714,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -746,7 +746,7 @@
         <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -778,7 +778,7 @@
         <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -811,7 +811,7 @@
         <v>53</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -844,7 +844,7 @@
         <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -877,7 +877,7 @@
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -909,7 +909,7 @@
         <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -941,7 +941,7 @@
         <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
         <v>11</v>
@@ -973,7 +973,7 @@
         <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1005,7 +1005,7 @@
         <v>53</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
@@ -1037,7 +1037,7 @@
         <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -1069,7 +1069,7 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" t="s">
         <v>15</v>
@@ -1101,7 +1101,7 @@
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -1133,7 +1133,7 @@
         <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -1165,7 +1165,7 @@
         <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -1197,7 +1197,7 @@
         <v>53</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -1229,7 +1229,7 @@
         <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s">
         <v>20</v>
@@ -1261,7 +1261,7 @@
         <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
@@ -1293,7 +1293,7 @@
         <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" t="s">
         <v>22</v>
@@ -1325,7 +1325,7 @@
         <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -1357,7 +1357,7 @@
         <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>24</v>
@@ -1389,7 +1389,7 @@
         <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
         <v>25</v>
@@ -1421,7 +1421,7 @@
         <v>53</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
         <v>26</v>
@@ -1453,7 +1453,7 @@
         <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
         <v>27</v>
@@ -1485,7 +1485,7 @@
         <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
         <v>28</v>
@@ -1517,7 +1517,7 @@
         <v>53</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
@@ -1549,7 +1549,7 @@
         <v>53</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
         <v>30</v>

</xml_diff>